<commit_message>
Correção ordem laços de repetição estratégia
</commit_message>
<xml_diff>
--- a/extracteds/Cases/Compra Fechamento Negativo - Select.xlsx
+++ b/extracteds/Cases/Compra Fechamento Negativo - Select.xlsx
@@ -525,7 +525,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +534,12 @@
     </fill>
     <fill>
       <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -549,15 +555,19 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="1" applyNumberFormat="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1044,86 +1054,86 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>126</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>27</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>27</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="5">
         <v>0.27570408064785212</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="5">
         <v>1.0211262246216745e-002</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="5">
         <v>2.2222222222222143e-002</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>323200</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="4">
         <v>1398037.3015873015</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>124</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>14</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>0.93333333333333335</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="5">
         <v>0.13549273762050057</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="5">
         <v>9.0328491747000382e-003</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="5">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="5">
         <v>2.0161290322580738e-002</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>1320900</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="4">
         <v>5386729.8387096776</v>
       </c>
     </row>
@@ -1172,46 +1182,46 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>124</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>23</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>20</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>0.86956521739130432</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="5">
         <v>0.1656617518199987</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="5">
         <v>7.2026848617390742e-003</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="5">
         <v>-1.3879250520471897e-002</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="5">
         <v>2.1577380952380931e-002</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>3179000</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="4">
         <v>10210191.935483871</v>
       </c>
     </row>
@@ -1260,46 +1270,46 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>124</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>21</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
         <v>0.91304347826086951</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="5">
         <v>0.22553412882964594</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="5">
         <v>9.8058316882454755e-003</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="5">
         <v>-1.6129032258064502e-002</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="5">
         <v>2.9702970297029729e-002</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>24885500</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="4">
         <v>81054071.774193555</v>
       </c>
     </row>
@@ -1788,46 +1798,46 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="4">
         <v>124</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>22</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>19</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="4">
         <v>3</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="5">
         <v>0.86363636363636365</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="5">
         <v>0.19126323203701964</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="5">
         <v>8.6937832744099844e-003</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="5">
         <v>-3.3703561853695829e-002</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="5">
         <v>3.5577658760520325e-002</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="4">
         <v>9086300</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="4">
         <v>20540425</v>
       </c>
     </row>
@@ -3768,433 +3778,433 @@
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
     </row>
     <row r="65" ht="14.25">
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
     </row>
     <row r="66" ht="14.25">
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
     </row>
     <row r="67" ht="14.25">
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="5"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
     </row>
     <row r="68" ht="14.25">
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
     </row>
     <row r="69" ht="14.25">
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
     </row>
     <row r="70" ht="14.25">
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
     </row>
     <row r="71" ht="14.25">
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
     </row>
     <row r="72" ht="14.25">
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
     </row>
     <row r="73" ht="14.25">
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
     </row>
     <row r="74" ht="14.25">
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
     </row>
     <row r="75" ht="14.25">
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
     </row>
     <row r="76" ht="14.25">
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
     </row>
     <row r="77" ht="14.25">
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
     </row>
     <row r="78" ht="14.25">
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
     </row>
     <row r="79" ht="14.25">
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
     </row>
     <row r="80" ht="14.25">
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
     </row>
     <row r="81" ht="14.25">
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
     </row>
     <row r="82" ht="14.25">
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
     </row>
     <row r="83" ht="14.25">
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
     </row>
     <row r="84" ht="14.25">
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
     </row>
     <row r="85" ht="14.25">
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
     </row>
     <row r="86" ht="14.25">
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
     </row>
     <row r="87" ht="14.25">
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
     </row>
     <row r="88" ht="14.25">
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
     </row>
     <row r="89" ht="14.25">
-      <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
-      <c r="I89" s="4"/>
-      <c r="J89" s="4"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
     </row>
     <row r="90" ht="14.25">
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
     </row>
     <row r="91" ht="14.25">
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
     </row>
     <row r="92" ht="14.25">
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
     </row>
     <row r="93" ht="14.25">
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
     </row>
     <row r="94" ht="14.25">
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
     </row>
     <row r="95" ht="14.25">
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
     </row>
     <row r="96" ht="14.25">
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
     </row>
     <row r="97" ht="14.25">
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
     </row>
     <row r="98" ht="14.25">
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="4"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
     </row>
     <row r="99" ht="14.25">
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
     </row>
     <row r="104" ht="14.25">
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
     </row>
     <row r="105" ht="14.25">
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="J105" s="4"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
     </row>
     <row r="106" ht="14.25">
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="4"/>
-      <c r="J106" s="4"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="4"/>
-      <c r="J107" s="4"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
     </row>
     <row r="108" ht="14.25">
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="4"/>
-      <c r="J108" s="4"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
     </row>
     <row r="109" ht="14.25">
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
-      <c r="J109" s="4"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
     </row>
     <row r="111" ht="14.25">
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
-      <c r="J111" s="4"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
     </row>
     <row r="112" ht="14.25">
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="4"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
     </row>
     <row r="113" ht="14.25">
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="4"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:N63" columnSort="0">

</xml_diff>